<commit_message>
new Sprint backlog 3 and 4
Changed Tasks in 3 and 4 Sprint Backlogs
</commit_message>
<xml_diff>
--- a/Doc/SprintBacklog3.xlsx
+++ b/Doc/SprintBacklog3.xlsx
@@ -123,12 +123,6 @@
     <t>answer chosen user`s question</t>
   </si>
   <si>
-    <t>As a user, I want to get an administration support</t>
-  </si>
-  <si>
-    <t>report administrator about my problems</t>
-  </si>
-  <si>
     <t>Day</t>
   </si>
   <si>
@@ -145,6 +139,12 @@
   </si>
   <si>
     <t>Burndown Chat Diagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As an admin, I want to  manage user list </t>
+  </si>
+  <si>
+    <t>delete a registrеd user</t>
   </si>
 </sst>
 </file>
@@ -777,48 +777,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -831,6 +789,48 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1000,11 +1000,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="181147136"/>
-        <c:axId val="181148672"/>
+        <c:axId val="146167296"/>
+        <c:axId val="146168832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="181147136"/>
+        <c:axId val="146167296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1013,7 +1013,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181148672"/>
+        <c:crossAx val="146168832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1021,7 +1021,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181148672"/>
+        <c:axId val="146168832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1032,7 +1032,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181147136"/>
+        <c:crossAx val="146167296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1378,8 +1378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1398,12 +1398,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1413,14 +1413,14 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="53"/>
+      <c r="D2" s="39"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -1430,14 +1430,14 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="55" t="s">
+      <c r="A3" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="40"/>
+      <c r="C3" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="55"/>
+      <c r="D3" s="41"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -1447,10 +1447,10 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -1495,7 +1495,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="48" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1530,7 +1530,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="A7" s="49"/>
       <c r="B7" s="4" t="s">
         <v>18</v>
       </c>
@@ -1563,7 +1563,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="50" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -1598,7 +1598,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="46"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
@@ -1631,7 +1631,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="52" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -1666,7 +1666,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="48"/>
+      <c r="A11" s="53"/>
       <c r="B11" s="6" t="s">
         <v>25</v>
       </c>
@@ -1699,7 +1699,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="54" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -1734,7 +1734,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
+      <c r="A13" s="55"/>
       <c r="B13" s="7" t="s">
         <v>28</v>
       </c>
@@ -1767,7 +1767,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="44" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -1802,7 +1802,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
+      <c r="A15" s="45"/>
       <c r="B15" s="8" t="s">
         <v>33</v>
       </c>
@@ -1835,7 +1835,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="8" t="s">
         <v>34</v>
       </c>
@@ -1869,10 +1869,10 @@
     </row>
     <row r="17" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>22</v>
@@ -1994,37 +1994,37 @@
       <c r="BB24" s="27"/>
     </row>
     <row r="25" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A25" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
+      <c r="A25" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
     </row>
     <row r="26" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A26" s="38"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
+      <c r="A26" s="43"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
     </row>
     <row r="28" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="C29" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="29" t="s">
+      <c r="F29" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="E29" s="29" t="s">
+      <c r="G29" s="31" t="s">
         <v>39</v>
-      </c>
-      <c r="F29" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="G29" s="31" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:54" x14ac:dyDescent="0.25">
@@ -2226,11 +2226,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
     <mergeCell ref="A25:E26"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A4:D4"/>
@@ -2238,6 +2233,11 @@
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>